<commit_message>
He creado dos nuevas clases una se encarga de obtener datos de un excel y la otra de crear graficos de barras, he creado un directorio de carpetas, son los equipos y los jugadores, y he creado un boton mas que crea una grafica actualiza de los puntos del jugador y lo guarda en su respectiva ccarpeta
</commit_message>
<xml_diff>
--- a/informe_AngelsLakers.xlsx
+++ b/informe_AngelsLakers.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="16">
   <si>
     <t>TCA</t>
   </si>
@@ -952,7 +952,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C3BCB7-CF2E-4DE1-9114-BE2911B154F0}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -960,7 +960,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -1192,44 +1192,73 @@
         <v>290</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="0">
-        <f t="shared" ref="A9:I9" si="0">AVERAGE(A2:A8)</f>
-        <v>181.85714285714286</v>
-      </c>
-      <c r="B9" s="0">
-        <f t="shared" si="0"/>
-        <v>31.714285714285715</v>
-      </c>
-      <c r="C9" s="0">
-        <f t="shared" si="0"/>
-        <v>201.28571428571428</v>
-      </c>
-      <c r="D9" s="0">
-        <f t="shared" si="0"/>
-        <v>80.285714285714292</v>
-      </c>
-      <c r="E9" s="0">
-        <f t="shared" si="0"/>
-        <v>474.14285714285717</v>
-      </c>
-      <c r="F9" s="0">
-        <f t="shared" si="0"/>
-        <v>96.391428571428577</v>
-      </c>
-      <c r="G9" s="0">
-        <f t="shared" si="0"/>
-        <v>114.30285714285715</v>
-      </c>
-      <c r="H9" s="0">
-        <f t="shared" si="0"/>
-        <v>111.28428571428572</v>
-      </c>
-      <c r="I9" s="0">
-        <f t="shared" si="0"/>
-        <v>459.42857142857144</v>
-      </c>
-      <c r="J9" t="s" s="0">
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>435.0</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>435.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>918.0</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>100.57</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <v>101.12</v>
+      </c>
+      <c r="I9" t="n" s="0">
+        <v>950.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <f>AVERAGE(A2:A9)</f>
+        <v>213.5</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <f>AVERAGE(B2:B9)</f>
+        <v>28.375</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <f>AVERAGE(C2:C9)</f>
+        <v>230.5</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <f>AVERAGE(D2:D9)</f>
+        <v>75.625</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <f>AVERAGE(E2:E9)</f>
+        <v>529.625</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <f>AVERAGE(F2:F9)</f>
+        <v>96.8425</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <f>AVERAGE(G2:G9)</f>
+        <v>112.58625</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <f>AVERAGE(H2:H9)</f>
+        <v>110.01375</v>
+      </c>
+      <c r="I10" t="n" s="0">
+        <f>AVERAGE(I2:I9)</f>
+        <v>520.75</v>
+      </c>
+      <c r="J10" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1486,41 +1515,41 @@
       <c r="A2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B2" s="0">
-        <f>'LeBron James'!A9</f>
-        <v>181.85714285714286</v>
-      </c>
-      <c r="C2" s="0">
-        <f>'LeBron James'!B9</f>
-        <v>31.714285714285715</v>
-      </c>
-      <c r="D2" s="0">
-        <f>'LeBron James'!C9</f>
-        <v>201.28571428571428</v>
-      </c>
-      <c r="E2" s="0">
-        <f>'LeBron James'!D9</f>
-        <v>80.285714285714292</v>
-      </c>
-      <c r="F2" s="0">
-        <f>'LeBron James'!E9</f>
-        <v>474.14285714285717</v>
-      </c>
-      <c r="G2" s="0">
-        <f>'LeBron James'!F9</f>
-        <v>96.391428571428577</v>
-      </c>
-      <c r="H2" s="0">
-        <f>'LeBron James'!G9</f>
-        <v>114.30285714285715</v>
-      </c>
-      <c r="I2" s="0">
-        <f>'LeBron James'!H9</f>
-        <v>111.28428571428572</v>
-      </c>
-      <c r="J2" s="0">
-        <f>'LeBron James'!I9</f>
-        <v>459.42857142857144</v>
+      <c r="B2" s="0" t="n">
+        <f>'LeBron James'!A10</f>
+        <v>213.5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f>'LeBron James'!B10</f>
+        <v>28.375</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f>'LeBron James'!C10</f>
+        <v>230.5</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f>'LeBron James'!D10</f>
+        <v>75.625</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f>'LeBron James'!E10</f>
+        <v>529.625</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f>'LeBron James'!F10</f>
+        <v>96.8425</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f>'LeBron James'!G10</f>
+        <v>112.58625</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f>'LeBron James'!H10</f>
+        <v>110.01375</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f>'LeBron James'!I10</f>
+        <v>520.75</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
He creado dos clases una que crea graficos combinados y otra que crea graficos de lineas, tambien he creado dos botonos que abren un jframe uno para los graficos de lineas y otra para el combinado
</commit_message>
<xml_diff>
--- a/informe_AngelsLakers.xlsx
+++ b/informe_AngelsLakers.xlsx
@@ -3,26 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walth\Documents\NetBeansProjects\InterfazBaloncesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA521EF-342C-4983-8F39-CE3D4764B89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F89560-8C0B-4CF6-A67F-570CAE9E7B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1788" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1788" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anthony Davis" sheetId="2" r:id="rId1"/>
     <sheet name="D Angelo Russell" sheetId="3" r:id="rId2"/>
     <sheet name="LeBron James" sheetId="4" r:id="rId3"/>
     <sheet name="Austin Reaves" sheetId="5" r:id="rId4"/>
-    <sheet name="final" sheetId="6" r:id="rId5"/>
-    <sheet name="Rui Hachimura" sheetId="7" r:id="rId6"/>
+    <sheet name="Rui Hachimura" sheetId="7" r:id="rId5"/>
+    <sheet name="final" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
   <si>
     <t>TCA</t>
   </si>
@@ -93,7 +93,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,246 +413,246 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>466</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>34</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>568</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>34</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>82.04</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>85.04</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>85.77</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>1016</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>436</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>4</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>538</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>34</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>910</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>81.040000000000006</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>81.41</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>82.28</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>926</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>57</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>57</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>43</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>158</v>
       </c>
-      <c r="F4" s="0">
-        <v>100</v>
-      </c>
-      <c r="G4" s="0">
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
         <v>110.53</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>104.06</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>57</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>57</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>43</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>158</v>
       </c>
-      <c r="F5" s="0">
-        <v>100</v>
-      </c>
-      <c r="G5" s="0">
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
         <v>110.53</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>104.06</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>47</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>110</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>102</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>42.73</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>44.55</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>45.63</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>63</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>43</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>63</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>45</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>214</v>
       </c>
-      <c r="F7" s="0">
-        <v>100</v>
-      </c>
-      <c r="G7" s="0">
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
         <v>134.13</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>129.22999999999999</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="0">
+      <c r="A8">
         <f t="shared" ref="A8:I8" si="0">AVERAGE(A2:A7)</f>
         <v>187.66666666666666</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>18.166666666666668</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>232.16666666666666</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>33.833333333333336</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>423.66666666666669</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>84.301666666666677</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>94.365000000000009</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>91.838333333333324</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>483.66666666666669</v>
       </c>
-      <c r="J8" t="s" s="0">
+      <c r="J8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -672,276 +671,276 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>540</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>850</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>80</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>1125</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>63.53</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>63.53</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>63.54</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>904</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>77</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>43</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>77</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>32</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>229</v>
       </c>
-      <c r="F3" s="0">
-        <v>100</v>
-      </c>
-      <c r="G3" s="0">
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
         <v>127.92</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>125.71</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>63</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>43</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>63</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>45</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>214</v>
       </c>
-      <c r="F4" s="0">
-        <v>100</v>
-      </c>
-      <c r="G4" s="0">
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
         <v>134.13</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>129.22999999999999</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>68</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>34</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>68</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>340</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>510</v>
       </c>
-      <c r="F5" s="0">
-        <v>100</v>
-      </c>
-      <c r="G5" s="0">
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
         <v>125</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>117.19</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>86</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>43</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>86</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>43</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>258</v>
       </c>
-      <c r="F6" s="0">
-        <v>100</v>
-      </c>
-      <c r="G6" s="0">
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
         <v>125</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>122.95</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>750</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>430</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>750</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>32</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>1962</v>
       </c>
-      <c r="F7" s="0">
-        <v>100</v>
-      </c>
-      <c r="G7" s="0">
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
         <v>128.66999999999999</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>128.38999999999999</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>1985</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n" s="0">
-        <v>420.0</v>
-      </c>
-      <c r="B8" t="n" s="0">
-        <v>210.0</v>
-      </c>
-      <c r="C8" t="n" s="0">
-        <v>420.0</v>
-      </c>
-      <c r="D8" t="n" s="0">
-        <v>21.0</v>
-      </c>
-      <c r="E8" t="n" s="0">
-        <v>1071.0</v>
-      </c>
-      <c r="F8" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="G8" t="n" s="0">
-        <v>125.0</v>
-      </c>
-      <c r="H8" t="n" s="0">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>420</v>
+      </c>
+      <c r="B8">
+        <v>210</v>
+      </c>
+      <c r="C8">
+        <v>420</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <v>1071</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>125</v>
+      </c>
+      <c r="H8">
         <v>124.76</v>
       </c>
-      <c r="I8" t="n" s="0">
-        <v>1071.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n" s="0">
-        <f>AVERAGE(A2:A8)</f>
-        <v>286.2857142857143</v>
-      </c>
-      <c r="B9" t="n" s="0">
-        <f>AVERAGE(B2:B8)</f>
+      <c r="I8">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" ref="A9:I9" si="0">AVERAGE(A2:A8)</f>
+        <v>286.28571428571428</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
         <v>114.71428571428571</v>
       </c>
-      <c r="C9" t="n" s="0">
-        <f>AVERAGE(C2:C8)</f>
+      <c r="C9">
+        <f t="shared" si="0"/>
         <v>330.57142857142856</v>
       </c>
-      <c r="D9" t="n" s="0">
-        <f>AVERAGE(D2:D8)</f>
-        <v>84.71428571428571</v>
-      </c>
-      <c r="E9" t="n" s="0">
-        <f>AVERAGE(E2:E8)</f>
-        <v>767.0</v>
-      </c>
-      <c r="F9" t="n" s="0">
-        <f>AVERAGE(F2:F8)</f>
-        <v>94.78999999999999</v>
-      </c>
-      <c r="G9" t="n" s="0">
-        <f>AVERAGE(G2:G8)</f>
-        <v>118.4642857142857</v>
-      </c>
-      <c r="H9" t="n" s="0">
-        <f>AVERAGE(H2:H8)</f>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>84.714285714285708</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>767</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>94.789999999999992</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>118.46428571428569</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
         <v>115.96714285714286</v>
       </c>
-      <c r="I9" t="n" s="0">
-        <f>AVERAGE(I2:I8)</f>
-        <v>746.2857142857143</v>
-      </c>
-      <c r="J9" t="s" s="0">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>746.28571428571433</v>
+      </c>
+      <c r="J9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -960,305 +959,305 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>432</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>466</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>34</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>898</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>92.7</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>92.7</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>93.35</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>466</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>34</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>568</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>34</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>1000</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>82.04</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>85.04</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>85.77</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>1016</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>57</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>57</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>43</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>158</v>
       </c>
-      <c r="F4" s="0">
-        <v>100</v>
-      </c>
-      <c r="G4" s="0">
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
         <v>110.53</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>104.06</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>101</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>56</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>101</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>23</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>281</v>
       </c>
-      <c r="F5" s="0">
-        <v>100</v>
-      </c>
-      <c r="G5" s="0">
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
         <v>127.72</v>
       </c>
-      <c r="H5" s="0">
+      <c r="H5">
         <v>126.44</v>
       </c>
-      <c r="I5" s="0">
+      <c r="I5">
         <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>63</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>43</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>63</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>45</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>214</v>
       </c>
-      <c r="F6" s="0">
-        <v>100</v>
-      </c>
-      <c r="G6" s="0">
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
         <v>134.13</v>
       </c>
-      <c r="H6" s="0">
+      <c r="H6">
         <v>129.22999999999999</v>
       </c>
-      <c r="I6" s="0">
+      <c r="I6">
         <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>68</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>34</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>68</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>340</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>510</v>
       </c>
-      <c r="F7" s="0">
-        <v>100</v>
-      </c>
-      <c r="G7" s="0">
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
         <v>125</v>
       </c>
-      <c r="H7" s="0">
+      <c r="H7">
         <v>117.19</v>
       </c>
-      <c r="I7" s="0">
+      <c r="I7">
         <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>86</v>
       </c>
-      <c r="B8" s="0">
+      <c r="B8">
         <v>43</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <v>86</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>43</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>258</v>
       </c>
-      <c r="F8" s="0">
-        <v>100</v>
-      </c>
-      <c r="G8" s="0">
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
         <v>125</v>
       </c>
-      <c r="H8" s="0">
+      <c r="H8">
         <v>122.95</v>
       </c>
-      <c r="I8" s="0">
+      <c r="I8">
         <v>290</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n" s="0">
-        <v>435.0</v>
-      </c>
-      <c r="B9" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="C9" t="n" s="0">
-        <v>435.0</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>43.0</v>
-      </c>
-      <c r="E9" t="n" s="0">
-        <v>918.0</v>
-      </c>
-      <c r="F9" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="G9" t="n" s="0">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>435</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>435</v>
+      </c>
+      <c r="D9">
+        <v>43</v>
+      </c>
+      <c r="E9">
+        <v>918</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
         <v>100.57</v>
       </c>
-      <c r="H9" t="n" s="0">
+      <c r="H9">
         <v>101.12</v>
       </c>
-      <c r="I9" t="n" s="0">
-        <v>950.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n" s="0">
-        <f>AVERAGE(A2:A9)</f>
+      <c r="I9">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" ref="A10:I10" si="0">AVERAGE(A2:A9)</f>
         <v>213.5</v>
       </c>
-      <c r="B10" t="n" s="0">
-        <f>AVERAGE(B2:B9)</f>
+      <c r="B10">
+        <f t="shared" si="0"/>
         <v>28.375</v>
       </c>
-      <c r="C10" t="n" s="0">
-        <f>AVERAGE(C2:C9)</f>
+      <c r="C10">
+        <f t="shared" si="0"/>
         <v>230.5</v>
       </c>
-      <c r="D10" t="n" s="0">
-        <f>AVERAGE(D2:D9)</f>
+      <c r="D10">
+        <f t="shared" si="0"/>
         <v>75.625</v>
       </c>
-      <c r="E10" t="n" s="0">
-        <f>AVERAGE(E2:E9)</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>529.625</v>
       </c>
-      <c r="F10" t="n" s="0">
-        <f>AVERAGE(F2:F9)</f>
-        <v>96.8425</v>
-      </c>
-      <c r="G10" t="n" s="0">
-        <f>AVERAGE(G2:G9)</f>
-        <v>112.58625</v>
-      </c>
-      <c r="H10" t="n" s="0">
-        <f>AVERAGE(H2:H9)</f>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>96.842500000000001</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>112.58625000000001</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
         <v>110.01375</v>
       </c>
-      <c r="I10" t="n" s="0">
-        <f>AVERAGE(I2:I9)</f>
+      <c r="I10">
+        <f t="shared" si="0"/>
         <v>520.75</v>
       </c>
-      <c r="J10" t="s" s="0">
+      <c r="J10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1275,189 +1274,189 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>466</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>34</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>568</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>34</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2">
         <v>1000</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2">
         <v>82.04</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>85.04</v>
       </c>
-      <c r="H2" s="0">
+      <c r="H2">
         <v>85.77</v>
       </c>
-      <c r="I2" s="0">
+      <c r="I2">
         <v>1016</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>77</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>43</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>487</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>34</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3">
         <v>231</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3">
         <v>15.81</v>
       </c>
-      <c r="G3" s="0">
+      <c r="G3">
         <v>20.23</v>
       </c>
-      <c r="H3" s="0">
+      <c r="H3">
         <v>23.01</v>
       </c>
-      <c r="I3" s="0">
+      <c r="I3">
         <v>-111</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>63</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>43</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>63</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>45</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>214</v>
       </c>
-      <c r="F4" s="0">
-        <v>100</v>
-      </c>
-      <c r="G4" s="0">
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
         <v>134.13</v>
       </c>
-      <c r="H4" s="0">
+      <c r="H4">
         <v>129.22999999999999</v>
       </c>
-      <c r="I4" s="0">
+      <c r="I4">
         <v>246</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>420.0</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>210.0</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>420.0</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>21.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>1071.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>125.0</v>
-      </c>
-      <c r="H5" t="n" s="0">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>420</v>
+      </c>
+      <c r="B5">
+        <v>210</v>
+      </c>
+      <c r="C5">
+        <v>420</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>1071</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>125</v>
+      </c>
+      <c r="H5">
         <v>124.76</v>
       </c>
-      <c r="I5" t="n" s="0">
-        <v>1071.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="0">
-        <f>AVERAGE(A2:A5)</f>
+      <c r="I5">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" ref="A6:I6" si="0">AVERAGE(A2:A5)</f>
         <v>256.5</v>
       </c>
-      <c r="B6" t="n" s="0">
-        <f>AVERAGE(B2:B5)</f>
+      <c r="B6">
+        <f t="shared" si="0"/>
         <v>82.5</v>
       </c>
-      <c r="C6" t="n" s="0">
-        <f>AVERAGE(C2:C5)</f>
+      <c r="C6">
+        <f t="shared" si="0"/>
         <v>384.5</v>
       </c>
-      <c r="D6" t="n" s="0">
-        <f>AVERAGE(D2:D5)</f>
+      <c r="D6">
+        <f t="shared" si="0"/>
         <v>33.5</v>
       </c>
-      <c r="E6" t="n" s="0">
-        <f>AVERAGE(E2:E5)</f>
-        <v>629.0</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <f>AVERAGE(F2:F5)</f>
-        <v>74.4625</v>
-      </c>
-      <c r="G6" t="n" s="0">
-        <f>AVERAGE(G2:G5)</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>629</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>74.462500000000006</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
         <v>91.1</v>
       </c>
-      <c r="H6" t="n" s="0">
-        <f>AVERAGE(H2:H5)</f>
-        <v>90.6925</v>
-      </c>
-      <c r="I6" t="n" s="0">
-        <f>AVERAGE(I2:I5)</f>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>90.692499999999995</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
         <v>555.5</v>
       </c>
-      <c r="J6" t="s" s="0">
+      <c r="J6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1467,253 +1466,110 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D05933-57D8-434E-87B0-F90FFDEDE176}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="15.88671875"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <f>'LeBron James'!A10</f>
-        <v>213.5</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <f>'LeBron James'!B10</f>
-        <v>28.375</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f>'LeBron James'!C10</f>
-        <v>230.5</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <f>'LeBron James'!D10</f>
-        <v>75.625</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <f>'LeBron James'!E10</f>
-        <v>529.625</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <f>'LeBron James'!F10</f>
-        <v>96.8425</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <f>'LeBron James'!G10</f>
-        <v>112.58625</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <f>'LeBron James'!H10</f>
-        <v>110.01375</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <f>'LeBron James'!I10</f>
-        <v>520.75</v>
+      <c r="A2">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>77</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>229</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>127.92</v>
+      </c>
+      <c r="H2">
+        <v>125.71</v>
+      </c>
+      <c r="I2">
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0">
-        <f>'Anthony Davis'!A8</f>
-        <v>187.66666666666666</v>
-      </c>
-      <c r="C3" s="0">
-        <f>'Anthony Davis'!B8</f>
-        <v>18.166666666666668</v>
-      </c>
-      <c r="D3" s="0">
-        <f>'Anthony Davis'!C8</f>
-        <v>232.16666666666666</v>
-      </c>
-      <c r="E3" s="0">
-        <f>'Anthony Davis'!D8</f>
-        <v>33.833333333333336</v>
-      </c>
-      <c r="F3" s="0">
-        <f>'Anthony Davis'!E8</f>
-        <v>423.66666666666669</v>
-      </c>
-      <c r="G3" s="0">
-        <f>'Anthony Davis'!F8</f>
-        <v>84.301666666666677</v>
-      </c>
-      <c r="H3" s="0">
-        <f>'Anthony Davis'!G8</f>
-        <v>94.365000000000009</v>
-      </c>
-      <c r="I3" s="0">
-        <f>'Anthony Davis'!H8</f>
-        <v>91.838333333333324</v>
-      </c>
-      <c r="J3" s="0">
-        <f>'Anthony Davis'!I8</f>
-        <v>483.66666666666669</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <f>'Austin Reaves'!A6</f>
-        <v>256.5</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <f>'Austin Reaves'!B6</f>
-        <v>82.5</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <f>'Austin Reaves'!C6</f>
-        <v>384.5</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <f>'Austin Reaves'!D6</f>
-        <v>33.5</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <f>'Austin Reaves'!E6</f>
-        <v>629.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <f>'Austin Reaves'!F6</f>
-        <v>74.4625</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <f>'Austin Reaves'!G6</f>
-        <v>91.1</v>
-      </c>
-      <c r="I4" t="n" s="0">
-        <f>'Austin Reaves'!H6</f>
-        <v>90.6925</v>
-      </c>
-      <c r="J4" t="n" s="0">
-        <f>'Austin Reaves'!I6</f>
-        <v>555.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <f>'D Angelo Russell'!A9</f>
-        <v>286.2857142857143</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <f>'D Angelo Russell'!B9</f>
-        <v>114.71428571428571</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <f>'D Angelo Russell'!C9</f>
-        <v>330.57142857142856</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <f>'D Angelo Russell'!D9</f>
-        <v>84.71428571428571</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <f>'D Angelo Russell'!E9</f>
-        <v>767.0</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <f>'D Angelo Russell'!F9</f>
-        <v>94.78999999999999</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <f>'D Angelo Russell'!G9</f>
-        <v>118.4642857142857</v>
-      </c>
-      <c r="I5" t="n" s="0">
-        <f>'D Angelo Russell'!H9</f>
-        <v>115.96714285714286</v>
-      </c>
-      <c r="J5" t="n" s="0">
-        <f>'D Angelo Russell'!I9</f>
-        <v>746.2857142857143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0">
-        <f>'Rui Hachimura'!A3</f>
+      <c r="A3">
+        <f t="shared" ref="A3:I3" si="0">AVERAGE(A2:A2)</f>
         <v>77</v>
       </c>
-      <c r="C6" s="0">
-        <f>'Rui Hachimura'!B3</f>
+      <c r="B3">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="D6" s="0">
-        <f>'Rui Hachimura'!C3</f>
+      <c r="C3">
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="E6" s="0">
-        <f>'Rui Hachimura'!D3</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="F6" s="0">
-        <f>'Rui Hachimura'!E3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>229</v>
       </c>
-      <c r="G6" s="0">
-        <f>'Rui Hachimura'!F3</f>
-        <v>100</v>
-      </c>
-      <c r="H6" s="0">
-        <f>'Rui Hachimura'!G3</f>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
         <v>127.92</v>
       </c>
-      <c r="I6" s="0">
-        <f>'Rui Hachimura'!H3</f>
+      <c r="H3">
+        <f t="shared" si="0"/>
         <v>125.71</v>
       </c>
-      <c r="J6" s="0">
-        <f>'Rui Hachimura'!I3</f>
+      <c r="I3">
+        <f t="shared" si="0"/>
         <v>261</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1722,110 +1578,253 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D05933-57D8-434E-87B0-F90FFDEDE176}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <f>'LeBron James'!A10</f>
+        <v>213.5</v>
+      </c>
+      <c r="C2">
+        <f>'LeBron James'!B10</f>
+        <v>28.375</v>
+      </c>
+      <c r="D2">
+        <f>'LeBron James'!C10</f>
+        <v>230.5</v>
+      </c>
+      <c r="E2">
+        <f>'LeBron James'!D10</f>
+        <v>75.625</v>
+      </c>
+      <c r="F2">
+        <f>'LeBron James'!E10</f>
+        <v>529.625</v>
+      </c>
+      <c r="G2">
+        <f>'LeBron James'!F10</f>
+        <v>96.842500000000001</v>
+      </c>
+      <c r="H2">
+        <f>'LeBron James'!G10</f>
+        <v>112.58625000000001</v>
+      </c>
+      <c r="I2">
+        <f>'LeBron James'!H10</f>
+        <v>110.01375</v>
+      </c>
+      <c r="J2">
+        <f>'LeBron James'!I10</f>
+        <v>520.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>'Anthony Davis'!A8</f>
+        <v>187.66666666666666</v>
+      </c>
+      <c r="C3">
+        <f>'Anthony Davis'!B8</f>
+        <v>18.166666666666668</v>
+      </c>
+      <c r="D3">
+        <f>'Anthony Davis'!C8</f>
+        <v>232.16666666666666</v>
+      </c>
+      <c r="E3">
+        <f>'Anthony Davis'!D8</f>
+        <v>33.833333333333336</v>
+      </c>
+      <c r="F3">
+        <f>'Anthony Davis'!E8</f>
+        <v>423.66666666666669</v>
+      </c>
+      <c r="G3">
+        <f>'Anthony Davis'!F8</f>
+        <v>84.301666666666677</v>
+      </c>
+      <c r="H3">
+        <f>'Anthony Davis'!G8</f>
+        <v>94.365000000000009</v>
+      </c>
+      <c r="I3">
+        <f>'Anthony Davis'!H8</f>
+        <v>91.838333333333324</v>
+      </c>
+      <c r="J3">
+        <f>'Anthony Davis'!I8</f>
+        <v>483.66666666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <f>'Austin Reaves'!A6</f>
+        <v>256.5</v>
+      </c>
+      <c r="C4">
+        <f>'Austin Reaves'!B6</f>
+        <v>82.5</v>
+      </c>
+      <c r="D4">
+        <f>'Austin Reaves'!C6</f>
+        <v>384.5</v>
+      </c>
+      <c r="E4">
+        <f>'Austin Reaves'!D6</f>
+        <v>33.5</v>
+      </c>
+      <c r="F4">
+        <f>'Austin Reaves'!E6</f>
+        <v>629</v>
+      </c>
+      <c r="G4">
+        <f>'Austin Reaves'!F6</f>
+        <v>74.462500000000006</v>
+      </c>
+      <c r="H4">
+        <f>'Austin Reaves'!G6</f>
+        <v>91.1</v>
+      </c>
+      <c r="I4">
+        <f>'Austin Reaves'!H6</f>
+        <v>90.692499999999995</v>
+      </c>
+      <c r="J4">
+        <f>'Austin Reaves'!I6</f>
+        <v>555.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>'D Angelo Russell'!A9</f>
+        <v>286.28571428571428</v>
+      </c>
+      <c r="C5">
+        <f>'D Angelo Russell'!B9</f>
+        <v>114.71428571428571</v>
+      </c>
+      <c r="D5">
+        <f>'D Angelo Russell'!C9</f>
+        <v>330.57142857142856</v>
+      </c>
+      <c r="E5">
+        <f>'D Angelo Russell'!D9</f>
+        <v>84.714285714285708</v>
+      </c>
+      <c r="F5">
+        <f>'D Angelo Russell'!E9</f>
+        <v>767</v>
+      </c>
+      <c r="G5">
+        <f>'D Angelo Russell'!F9</f>
+        <v>94.789999999999992</v>
+      </c>
+      <c r="H5">
+        <f>'D Angelo Russell'!G9</f>
+        <v>118.46428571428569</v>
+      </c>
+      <c r="I5">
+        <f>'D Angelo Russell'!H9</f>
+        <v>115.96714285714286</v>
+      </c>
+      <c r="J5">
+        <f>'D Angelo Russell'!I9</f>
+        <v>746.28571428571433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <f>'Rui Hachimura'!A3</f>
         <v>77</v>
       </c>
-      <c r="B2" s="0">
+      <c r="C6">
+        <f>'Rui Hachimura'!B3</f>
         <v>43</v>
       </c>
-      <c r="C2" s="0">
+      <c r="D6">
+        <f>'Rui Hachimura'!C3</f>
         <v>77</v>
       </c>
-      <c r="D2" s="0">
+      <c r="E6">
+        <f>'Rui Hachimura'!D3</f>
         <v>32</v>
       </c>
-      <c r="E2" s="0">
+      <c r="F6">
+        <f>'Rui Hachimura'!E3</f>
         <v>229</v>
       </c>
-      <c r="F2" s="0">
-        <v>100</v>
-      </c>
-      <c r="G2" s="0">
+      <c r="G6">
+        <f>'Rui Hachimura'!F3</f>
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <f>'Rui Hachimura'!G3</f>
         <v>127.92</v>
       </c>
-      <c r="H2" s="0">
+      <c r="I6">
+        <f>'Rui Hachimura'!H3</f>
         <v>125.71</v>
       </c>
-      <c r="I2" s="0">
+      <c r="J6">
+        <f>'Rui Hachimura'!I3</f>
         <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
-        <f t="shared" ref="A3:I3" si="0">AVERAGE(A2:A2)</f>
-        <v>77</v>
-      </c>
-      <c r="B3" s="0">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="C3" s="0">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="D3" s="0">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="E3" s="0">
-        <f t="shared" si="0"/>
-        <v>229</v>
-      </c>
-      <c r="F3" s="0">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G3" s="0">
-        <f t="shared" si="0"/>
-        <v>127.92</v>
-      </c>
-      <c r="H3" s="0">
-        <f t="shared" si="0"/>
-        <v>125.71</v>
-      </c>
-      <c r="I3" s="0">
-        <f t="shared" si="0"/>
-        <v>261</v>
-      </c>
-      <c r="J3" t="s" s="0">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Simplemente he refactorizado la clase InterfazBaloncesto y he añadido algún que otro comentario para que se entienda mejor la clase
</commit_message>
<xml_diff>
--- a/informe_AngelsLakers.xlsx
+++ b/informe_AngelsLakers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walth\Documents\NetBeansProjects\InterfazBaloncesto\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="16">
   <si>
     <t>TCA</t>
   </si>
@@ -93,6 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,246 +414,246 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>466</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>34</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>568</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>34</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1000</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>82.04</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>85.04</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>85.77</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>1016</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>436</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>538</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>34</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>910</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>81.040000000000006</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>81.41</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>82.28</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>926</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>57</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>43</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>158</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>110.53</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>104.06</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>57</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>57</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>43</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>158</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>110.53</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>104.06</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>47</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>110</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>102</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>42.73</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>44.55</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>45.63</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>63</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>43</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>63</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>45</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>214</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>100</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>134.13</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>129.22999999999999</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="0">
         <f t="shared" ref="A8:I8" si="0">AVERAGE(A2:A7)</f>
         <v>187.66666666666666</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <f t="shared" si="0"/>
         <v>18.166666666666668</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <f t="shared" si="0"/>
         <v>232.16666666666666</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <f t="shared" si="0"/>
         <v>33.833333333333336</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <f t="shared" si="0"/>
         <v>423.66666666666669</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <f t="shared" si="0"/>
         <v>84.301666666666677</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <f t="shared" si="0"/>
         <v>94.365000000000009</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <f t="shared" si="0"/>
         <v>91.838333333333324</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <f t="shared" si="0"/>
         <v>483.66666666666669</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -672,275 +673,275 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>540</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>850</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>80</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1125</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>63.53</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>63.53</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>63.54</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>904</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>77</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>43</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>77</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>32</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>229</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>100</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>127.92</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>125.71</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>63</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>43</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>63</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>45</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>214</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>134.13</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>129.22999999999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>68</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>34</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>68</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>340</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>510</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>125</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>117.19</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>86</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>43</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>86</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>43</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>258</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>100</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>125</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>122.95</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>750</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>430</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>750</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>32</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>1962</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>100</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>128.66999999999999</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>128.38999999999999</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>1985</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>420</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>210</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>420</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>21</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>1071</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>100</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>125</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>124.76</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>1071</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="0">
         <f t="shared" ref="A9:I9" si="0">AVERAGE(A2:A8)</f>
         <v>286.28571428571428</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <f t="shared" si="0"/>
         <v>114.71428571428571</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <f t="shared" si="0"/>
         <v>330.57142857142856</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <f t="shared" si="0"/>
         <v>84.714285714285708</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <f t="shared" si="0"/>
         <v>767</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <f t="shared" si="0"/>
         <v>94.789999999999992</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <f t="shared" si="0"/>
         <v>118.46428571428569</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <f t="shared" si="0"/>
         <v>115.96714285714286</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <f t="shared" si="0"/>
         <v>746.28571428571433</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -960,304 +961,304 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>432</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>466</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>34</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>898</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>92.7</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>92.7</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>93.35</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>466</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>34</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>568</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>34</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>1000</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>82.04</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>85.04</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>85.77</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>1016</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>57</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>43</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>158</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>110.53</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>104.06</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>101</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>56</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>101</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>23</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>281</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>127.72</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>126.44</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>63</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>43</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>63</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>45</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>214</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>100</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>134.13</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <v>129.22999999999999</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>68</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>34</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>68</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>340</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>510</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>100</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>125</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="0">
         <v>117.19</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="0">
         <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>86</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>43</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>86</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>43</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>258</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>100</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>125</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="0">
         <v>122.95</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="0">
         <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>435</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>435</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>43</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>918</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>100</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>100.57</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="0">
         <v>101.12</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="0">
         <v>950</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="0">
         <f t="shared" ref="A10:I10" si="0">AVERAGE(A2:A9)</f>
         <v>213.5</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <f t="shared" si="0"/>
         <v>28.375</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <f t="shared" si="0"/>
         <v>230.5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <f t="shared" si="0"/>
         <v>75.625</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="0">
         <f t="shared" si="0"/>
         <v>529.625</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <f t="shared" si="0"/>
         <v>96.842500000000001</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <f t="shared" si="0"/>
         <v>112.58625000000001</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="0">
         <f t="shared" si="0"/>
         <v>110.01375</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="0">
         <f t="shared" si="0"/>
         <v>520.75</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1275,188 +1276,188 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>466</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>34</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>568</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>34</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>1000</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>82.04</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>85.04</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>85.77</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>1016</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>77</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>43</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>487</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>34</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <v>231</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>15.81</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <v>20.23</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <v>23.01</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <v>-111</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>63</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>43</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>63</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>45</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>214</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>134.13</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <v>129.22999999999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>420</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>210</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>420</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>21</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>1071</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>125</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <v>124.76</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <v>1071</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="0">
         <f t="shared" ref="A6:I6" si="0">AVERAGE(A2:A5)</f>
         <v>256.5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <f t="shared" si="0"/>
         <v>82.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <f t="shared" si="0"/>
         <v>384.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <f t="shared" si="0"/>
         <v>33.5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <f t="shared" si="0"/>
         <v>629</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <f t="shared" si="0"/>
         <v>74.462500000000006</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <f t="shared" si="0"/>
         <v>91.1</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="0">
         <f t="shared" si="0"/>
         <v>90.692499999999995</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="0">
         <f t="shared" si="0"/>
         <v>555.5</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1467,108 +1468,137 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>77</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>43</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>77</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>32</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <v>229</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>100</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>127.92</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <v>125.71</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <f t="shared" ref="A3:I3" si="0">AVERAGE(A2:A2)</f>
-        <v>77</v>
-      </c>
-      <c r="B3">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>229</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>127.92</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>125.71</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>261</v>
-      </c>
-      <c r="J3" t="s">
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>550.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>277.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>161.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>9.09</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>9.55</v>
+      </c>
+      <c r="H3" t="n" s="0">
+        <v>11.98</v>
+      </c>
+      <c r="I3" t="n" s="0">
+        <v>-511.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <f>AVERAGE(A2:A3)</f>
+        <v>63.5</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <f>AVERAGE(B2:B3)</f>
+        <v>24.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <f>AVERAGE(C2:C3)</f>
+        <v>313.5</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <f>AVERAGE(D2:D3)</f>
+        <v>154.5</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <f>AVERAGE(E2:E3)</f>
+        <v>195.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <f>AVERAGE(F2:F3)</f>
+        <v>54.545</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <f>AVERAGE(G2:G3)</f>
+        <v>68.735</v>
+      </c>
+      <c r="H4" t="n" s="0">
+        <f>AVERAGE(H2:H3)</f>
+        <v>68.845</v>
+      </c>
+      <c r="I4" t="n" s="0">
+        <f>AVERAGE(I2:I3)</f>
+        <v>-125.0</v>
+      </c>
+      <c r="J4" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1587,244 +1617,244 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <f>'LeBron James'!A10</f>
         <v>213.5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <f>'LeBron James'!B10</f>
         <v>28.375</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <f>'LeBron James'!C10</f>
         <v>230.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="0">
         <f>'LeBron James'!D10</f>
         <v>75.625</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <f>'LeBron James'!E10</f>
         <v>529.625</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <f>'LeBron James'!F10</f>
         <v>96.842500000000001</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="0">
         <f>'LeBron James'!G10</f>
         <v>112.58625000000001</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="0">
         <f>'LeBron James'!H10</f>
         <v>110.01375</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="0">
         <f>'LeBron James'!I10</f>
         <v>520.75</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <f>'Anthony Davis'!A8</f>
         <v>187.66666666666666</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <f>'Anthony Davis'!B8</f>
         <v>18.166666666666668</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <f>'Anthony Davis'!C8</f>
         <v>232.16666666666666</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="0">
         <f>'Anthony Davis'!D8</f>
         <v>33.833333333333336</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <f>'Anthony Davis'!E8</f>
         <v>423.66666666666669</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="0">
         <f>'Anthony Davis'!F8</f>
         <v>84.301666666666677</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="0">
         <f>'Anthony Davis'!G8</f>
         <v>94.365000000000009</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="0">
         <f>'Anthony Davis'!H8</f>
         <v>91.838333333333324</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="0">
         <f>'Anthony Davis'!I8</f>
         <v>483.66666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <f>'Austin Reaves'!A6</f>
         <v>256.5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <f>'Austin Reaves'!B6</f>
         <v>82.5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <f>'Austin Reaves'!C6</f>
         <v>384.5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <f>'Austin Reaves'!D6</f>
         <v>33.5</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <f>'Austin Reaves'!E6</f>
         <v>629</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <f>'Austin Reaves'!F6</f>
         <v>74.462500000000006</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="0">
         <f>'Austin Reaves'!G6</f>
         <v>91.1</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <f>'Austin Reaves'!H6</f>
         <v>90.692499999999995</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="0">
         <f>'Austin Reaves'!I6</f>
         <v>555.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <f>'D Angelo Russell'!A9</f>
         <v>286.28571428571428</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <f>'D Angelo Russell'!B9</f>
         <v>114.71428571428571</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <f>'D Angelo Russell'!C9</f>
         <v>330.57142857142856</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <f>'D Angelo Russell'!D9</f>
         <v>84.714285714285708</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <f>'D Angelo Russell'!E9</f>
         <v>767</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <f>'D Angelo Russell'!F9</f>
         <v>94.789999999999992</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="0">
         <f>'D Angelo Russell'!G9</f>
         <v>118.46428571428569</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="0">
         <f>'D Angelo Russell'!H9</f>
         <v>115.96714285714286</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="0">
         <f>'D Angelo Russell'!I9</f>
         <v>746.28571428571433</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B6">
-        <f>'Rui Hachimura'!A3</f>
-        <v>77</v>
-      </c>
-      <c r="C6">
-        <f>'Rui Hachimura'!B3</f>
-        <v>43</v>
-      </c>
-      <c r="D6">
-        <f>'Rui Hachimura'!C3</f>
-        <v>77</v>
-      </c>
-      <c r="E6">
-        <f>'Rui Hachimura'!D3</f>
-        <v>32</v>
-      </c>
-      <c r="F6">
-        <f>'Rui Hachimura'!E3</f>
-        <v>229</v>
-      </c>
-      <c r="G6">
-        <f>'Rui Hachimura'!F3</f>
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <f>'Rui Hachimura'!G3</f>
-        <v>127.92</v>
-      </c>
-      <c r="I6">
-        <f>'Rui Hachimura'!H3</f>
-        <v>125.71</v>
-      </c>
-      <c r="J6">
-        <f>'Rui Hachimura'!I3</f>
-        <v>261</v>
+      <c r="B6" t="n" s="0">
+        <f>'Rui Hachimura'!A4</f>
+        <v>63.5</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <f>'Rui Hachimura'!B4</f>
+        <v>24.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <f>'Rui Hachimura'!C4</f>
+        <v>313.5</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <f>'Rui Hachimura'!D4</f>
+        <v>154.5</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <f>'Rui Hachimura'!E4</f>
+        <v>195.0</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <f>'Rui Hachimura'!F4</f>
+        <v>54.545</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <f>'Rui Hachimura'!G4</f>
+        <v>68.735</v>
+      </c>
+      <c r="I6" t="n" s="0">
+        <f>'Rui Hachimura'!H4</f>
+        <v>68.845</v>
+      </c>
+      <c r="J6" t="n" s="0">
+        <f>'Rui Hachimura'!I4</f>
+        <v>-125.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
He creado una clase mas que DataInPdf, que lo que hace esto es poner datos que le paso por parametros y exportar los datos en un pdf que he creado, y puede abrir el archivo
</commit_message>
<xml_diff>
--- a/informe_AngelsLakers.xlsx
+++ b/informe_AngelsLakers.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="16">
   <si>
     <t>TCA</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D1ED6-C4A2-4C22-BEF0-2BCF567880B1}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
@@ -413,7 +413,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -616,44 +616,73 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="0">
-        <f t="shared" ref="A8:I8" si="0">AVERAGE(A2:A7)</f>
-        <v>187.66666666666666</v>
-      </c>
-      <c r="B8" s="0">
-        <f t="shared" si="0"/>
-        <v>18.166666666666668</v>
-      </c>
-      <c r="C8" s="0">
-        <f t="shared" si="0"/>
-        <v>232.16666666666666</v>
-      </c>
-      <c r="D8" s="0">
-        <f t="shared" si="0"/>
-        <v>33.833333333333336</v>
-      </c>
-      <c r="E8" s="0">
-        <f t="shared" si="0"/>
-        <v>423.66666666666669</v>
-      </c>
-      <c r="F8" s="0">
-        <f t="shared" si="0"/>
-        <v>84.301666666666677</v>
-      </c>
-      <c r="G8" s="0">
-        <f t="shared" si="0"/>
-        <v>94.365000000000009</v>
-      </c>
-      <c r="H8" s="0">
-        <f t="shared" si="0"/>
-        <v>91.838333333333324</v>
-      </c>
-      <c r="I8" s="0">
-        <f t="shared" si="0"/>
-        <v>483.66666666666669</v>
-      </c>
-      <c r="J8" t="s" s="0">
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>363.0</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>456.0</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>781.0</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>79.61</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>84.32</v>
+      </c>
+      <c r="H8" t="n" s="0">
+        <v>84.66</v>
+      </c>
+      <c r="I8" t="n" s="0">
+        <v>782.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <f>AVERAGE(A2:A8)</f>
+        <v>212.71428571428572</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <f>AVERAGE(B2:B8)</f>
+        <v>21.714285714285715</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <f>AVERAGE(C2:C8)</f>
+        <v>264.14285714285717</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <f>AVERAGE(D2:D8)</f>
+        <v>30.714285714285715</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <f>AVERAGE(E2:E8)</f>
+        <v>474.7142857142857</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <f>AVERAGE(F2:F8)</f>
+        <v>83.63142857142859</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <f>AVERAGE(G2:G8)</f>
+        <v>92.92999999999999</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <f>AVERAGE(H2:H8)</f>
+        <v>90.81285714285714</v>
+      </c>
+      <c r="I9" t="n" s="0">
+        <f>AVERAGE(I2:I8)</f>
+        <v>526.2857142857143</v>
+      </c>
+      <c r="J9" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -664,7 +693,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9BD210-1F2D-417D-B3BC-A4A55EA866E3}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
@@ -672,7 +701,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -904,44 +933,131 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="0">
-        <f t="shared" ref="A9:I9" si="0">AVERAGE(A2:A8)</f>
-        <v>286.28571428571428</v>
-      </c>
-      <c r="B9" s="0">
-        <f t="shared" si="0"/>
-        <v>114.71428571428571</v>
-      </c>
-      <c r="C9" s="0">
-        <f t="shared" si="0"/>
-        <v>330.57142857142856</v>
-      </c>
-      <c r="D9" s="0">
-        <f t="shared" si="0"/>
-        <v>84.714285714285708</v>
-      </c>
-      <c r="E9" s="0">
-        <f t="shared" si="0"/>
-        <v>767</v>
-      </c>
-      <c r="F9" s="0">
-        <f t="shared" si="0"/>
-        <v>94.789999999999992</v>
-      </c>
-      <c r="G9" s="0">
-        <f t="shared" si="0"/>
-        <v>118.46428571428569</v>
-      </c>
-      <c r="H9" s="0">
-        <f t="shared" si="0"/>
-        <v>115.96714285714286</v>
-      </c>
-      <c r="I9" s="0">
-        <f t="shared" si="0"/>
-        <v>746.28571428571433</v>
-      </c>
-      <c r="J9" t="s" s="0">
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>150.0</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>330.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>330.0</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>45.45</v>
+      </c>
+      <c r="G9" t="n" s="0">
+        <v>46.21</v>
+      </c>
+      <c r="H9" t="n" s="0">
+        <v>48.39</v>
+      </c>
+      <c r="I9" t="n" s="0">
+        <v>202.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>79.0</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>140.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>215.0</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>56.43</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>72.5</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>72.24</v>
+      </c>
+      <c r="I10" t="n" s="0">
+        <v>186.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>79.0</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>140.0</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>215.0</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>56.43</v>
+      </c>
+      <c r="G11" t="n" s="0">
+        <v>72.5</v>
+      </c>
+      <c r="H11" t="n" s="0">
+        <v>72.24</v>
+      </c>
+      <c r="I11" t="n" s="0">
+        <v>186.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <f>AVERAGE(A2:A11)</f>
+        <v>231.2</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <f>AVERAGE(B2:B11)</f>
+        <v>89.8</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <f>AVERAGE(C2:C11)</f>
+        <v>292.4</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <f>AVERAGE(D2:D11)</f>
+        <v>65.8</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <f>AVERAGE(E2:E11)</f>
+        <v>612.9</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <f>AVERAGE(F2:F11)</f>
+        <v>82.184</v>
+      </c>
+      <c r="G12" t="n" s="0">
+        <f>AVERAGE(G2:G11)</f>
+        <v>102.04599999999999</v>
+      </c>
+      <c r="H12" t="n" s="0">
+        <f>AVERAGE(H2:H11)</f>
+        <v>100.464</v>
+      </c>
+      <c r="I12" t="n" s="0">
+        <f>AVERAGE(I2:I11)</f>
+        <v>579.8</v>
+      </c>
+      <c r="J12" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1697,41 +1813,41 @@
       <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3" s="0">
-        <f>'Anthony Davis'!A8</f>
-        <v>187.66666666666666</v>
-      </c>
-      <c r="C3" s="0">
-        <f>'Anthony Davis'!B8</f>
-        <v>18.166666666666668</v>
-      </c>
-      <c r="D3" s="0">
-        <f>'Anthony Davis'!C8</f>
-        <v>232.16666666666666</v>
-      </c>
-      <c r="E3" s="0">
-        <f>'Anthony Davis'!D8</f>
-        <v>33.833333333333336</v>
-      </c>
-      <c r="F3" s="0">
-        <f>'Anthony Davis'!E8</f>
-        <v>423.66666666666669</v>
-      </c>
-      <c r="G3" s="0">
-        <f>'Anthony Davis'!F8</f>
-        <v>84.301666666666677</v>
-      </c>
-      <c r="H3" s="0">
-        <f>'Anthony Davis'!G8</f>
-        <v>94.365000000000009</v>
-      </c>
-      <c r="I3" s="0">
-        <f>'Anthony Davis'!H8</f>
-        <v>91.838333333333324</v>
-      </c>
-      <c r="J3" s="0">
-        <f>'Anthony Davis'!I8</f>
-        <v>483.66666666666669</v>
+      <c r="B3" s="0" t="n">
+        <f>'Anthony Davis'!A9</f>
+        <v>212.71428571428572</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <f>'Anthony Davis'!B9</f>
+        <v>21.714285714285715</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f>'Anthony Davis'!C9</f>
+        <v>264.14285714285717</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f>'Anthony Davis'!D9</f>
+        <v>30.714285714285715</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f>'Anthony Davis'!E9</f>
+        <v>474.7142857142857</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f>'Anthony Davis'!F9</f>
+        <v>83.63142857142859</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f>'Anthony Davis'!G9</f>
+        <v>92.92999999999999</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f>'Anthony Davis'!H9</f>
+        <v>90.81285714285714</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f>'Anthony Davis'!I9</f>
+        <v>526.2857142857143</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1779,41 +1895,41 @@
       <c r="A5" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B5" s="0">
-        <f>'D Angelo Russell'!A9</f>
-        <v>286.28571428571428</v>
-      </c>
-      <c r="C5" s="0">
-        <f>'D Angelo Russell'!B9</f>
-        <v>114.71428571428571</v>
-      </c>
-      <c r="D5" s="0">
-        <f>'D Angelo Russell'!C9</f>
-        <v>330.57142857142856</v>
-      </c>
-      <c r="E5" s="0">
-        <f>'D Angelo Russell'!D9</f>
-        <v>84.714285714285708</v>
-      </c>
-      <c r="F5" s="0">
-        <f>'D Angelo Russell'!E9</f>
-        <v>767</v>
-      </c>
-      <c r="G5" s="0">
-        <f>'D Angelo Russell'!F9</f>
-        <v>94.789999999999992</v>
-      </c>
-      <c r="H5" s="0">
-        <f>'D Angelo Russell'!G9</f>
-        <v>118.46428571428569</v>
-      </c>
-      <c r="I5" s="0">
-        <f>'D Angelo Russell'!H9</f>
-        <v>115.96714285714286</v>
-      </c>
-      <c r="J5" s="0">
-        <f>'D Angelo Russell'!I9</f>
-        <v>746.28571428571433</v>
+      <c r="B5" s="0" t="n">
+        <f>'D Angelo Russell'!A12</f>
+        <v>231.2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <f>'D Angelo Russell'!B12</f>
+        <v>89.8</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f>'D Angelo Russell'!C12</f>
+        <v>292.4</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f>'D Angelo Russell'!D12</f>
+        <v>65.8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <f>'D Angelo Russell'!E12</f>
+        <v>612.9</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f>'D Angelo Russell'!F12</f>
+        <v>82.184</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f>'D Angelo Russell'!G12</f>
+        <v>102.04599999999999</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f>'D Angelo Russell'!H12</f>
+        <v>100.464</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f>'D Angelo Russell'!I12</f>
+        <v>579.8</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
He creado un componente con 3 tipos de cambio de tamaño de la letra, tambien he creado otra clase que es un segundo jframe para añadir cosas, y finalmente he cambiado la interfaz grafica, he puesto el componente y los diferentes pantallas.
</commit_message>
<xml_diff>
--- a/informe_AngelsLakers.xlsx
+++ b/informe_AngelsLakers.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="16">
   <si>
     <t>TCA</t>
   </si>
@@ -1385,13 +1385,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -1536,44 +1536,73 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
-        <f t="shared" ref="A6:I6" si="0">AVERAGE(A2:A5)</f>
-        <v>256.5</v>
-      </c>
-      <c r="B6" s="0">
-        <f t="shared" si="0"/>
-        <v>82.5</v>
-      </c>
-      <c r="C6" s="0">
-        <f t="shared" si="0"/>
-        <v>384.5</v>
-      </c>
-      <c r="D6" s="0">
-        <f t="shared" si="0"/>
-        <v>33.5</v>
-      </c>
-      <c r="E6" s="0">
-        <f t="shared" si="0"/>
-        <v>629</v>
-      </c>
-      <c r="F6" s="0">
-        <f t="shared" si="0"/>
-        <v>74.462500000000006</v>
-      </c>
-      <c r="G6" s="0">
-        <f t="shared" si="0"/>
-        <v>91.1</v>
-      </c>
-      <c r="H6" s="0">
-        <f t="shared" si="0"/>
-        <v>90.692499999999995</v>
-      </c>
-      <c r="I6" s="0">
-        <f t="shared" si="0"/>
-        <v>555.5</v>
-      </c>
-      <c r="J6" t="s" s="0">
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>140.0</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>320.0</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>563.0</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>71.43</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>86.79</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <v>100.25</v>
+      </c>
+      <c r="I6" t="n" s="0">
+        <v>507.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <f>AVERAGE(A2:A6)</f>
+        <v>225.2</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <f>AVERAGE(B2:B6)</f>
+        <v>74.6</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <f>AVERAGE(C2:C6)</f>
+        <v>335.6</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <f>AVERAGE(D2:D6)</f>
+        <v>90.8</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <f>AVERAGE(E2:E6)</f>
+        <v>615.8</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <f>AVERAGE(F2:F6)</f>
+        <v>73.85600000000001</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <f>AVERAGE(G2:G6)</f>
+        <v>90.238</v>
+      </c>
+      <c r="H7" t="n" s="0">
+        <f>AVERAGE(H2:H6)</f>
+        <v>92.604</v>
+      </c>
+      <c r="I7" t="n" s="0">
+        <f>AVERAGE(I2:I6)</f>
+        <v>545.8</v>
+      </c>
+      <c r="J7" t="s" s="0">
         <v>9</v>
       </c>
     </row>
@@ -1854,41 +1883,41 @@
       <c r="A4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B4" s="0">
-        <f>'Austin Reaves'!A6</f>
-        <v>256.5</v>
-      </c>
-      <c r="C4" s="0">
-        <f>'Austin Reaves'!B6</f>
-        <v>82.5</v>
-      </c>
-      <c r="D4" s="0">
-        <f>'Austin Reaves'!C6</f>
-        <v>384.5</v>
-      </c>
-      <c r="E4" s="0">
-        <f>'Austin Reaves'!D6</f>
-        <v>33.5</v>
-      </c>
-      <c r="F4" s="0">
-        <f>'Austin Reaves'!E6</f>
-        <v>629</v>
-      </c>
-      <c r="G4" s="0">
-        <f>'Austin Reaves'!F6</f>
-        <v>74.462500000000006</v>
-      </c>
-      <c r="H4" s="0">
-        <f>'Austin Reaves'!G6</f>
-        <v>91.1</v>
-      </c>
-      <c r="I4" s="0">
-        <f>'Austin Reaves'!H6</f>
-        <v>90.692499999999995</v>
-      </c>
-      <c r="J4" s="0">
-        <f>'Austin Reaves'!I6</f>
-        <v>555.5</v>
+      <c r="B4" s="0" t="n">
+        <f>'Austin Reaves'!A7</f>
+        <v>225.2</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f>'Austin Reaves'!B7</f>
+        <v>74.6</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f>'Austin Reaves'!C7</f>
+        <v>335.6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f>'Austin Reaves'!D7</f>
+        <v>90.8</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f>'Austin Reaves'!E7</f>
+        <v>615.8</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f>'Austin Reaves'!F7</f>
+        <v>73.85600000000001</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f>'Austin Reaves'!G7</f>
+        <v>90.238</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f>'Austin Reaves'!H7</f>
+        <v>92.604</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f>'Austin Reaves'!I7</f>
+        <v>545.8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>